<commit_message>
Run on dask or multiprocessing
</commit_message>
<xml_diff>
--- a/results/SDGym-Leaderboard.xlsx
+++ b/results/SDGym-Leaderboard.xlsx
@@ -8,22 +8,38 @@
   </bookViews>
   <sheets>
     <sheet name="Number of wins per version" sheetId="1" r:id="rId1"/>
-    <sheet name="0.2.1" sheetId="2" r:id="rId2"/>
-    <sheet name="0.2.0" sheetId="3" r:id="rId3"/>
+    <sheet name="0.2.2.dev0" sheetId="2" r:id="rId2"/>
+    <sheet name="0.2.1" sheetId="3" r:id="rId3"/>
+    <sheet name="0.2.0" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="42">
   <si>
     <t>CLBNSynthesizer</t>
   </si>
   <si>
+    <t>CTGAN</t>
+  </si>
+  <si>
     <t>CTGANSynthesizer</t>
   </si>
   <si>
+    <t>CopulaGAN</t>
+  </si>
+  <si>
+    <t>GaussianCopulaCategorical</t>
+  </si>
+  <si>
+    <t>GaussianCopulaCategoricalFuzzy</t>
+  </si>
+  <si>
+    <t>GaussianCopulaOneHot</t>
+  </si>
+  <si>
     <t>MedganSynthesizer</t>
   </si>
   <si>
@@ -39,10 +55,16 @@
     <t>VEEGANSynthesizer</t>
   </si>
   <si>
+    <t>N/E</t>
+  </si>
+  <si>
     <t>Gaussian Mixture Simulated Data</t>
   </si>
   <si>
     <t>Synthesizer</t>
+  </si>
+  <si>
+    <t>0.2.2.dev0</t>
   </si>
   <si>
     <t>0.2.1</t>
@@ -477,34 +499,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,21 +538,27 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -536,234 +568,507 @@
       <c r="C5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="2">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="2">
         <v>5</v>
       </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="C42" s="2">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="2">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="2">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
         <v>0</v>
       </c>
     </row>
@@ -774,7 +1079,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -791,35 +1096,35 @@
     <col min="9" max="9" width="27.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,9 +1147,9 @@
         <v>-18.90481475924042</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>-9.162882145624636</v>
@@ -865,9 +1170,9 @@
         <v>-2.737148674403763</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>-6.833268269910192</v>
@@ -888,9 +1193,9 @@
         <v>-133.4629003196207</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>-6.777963983549516</v>
@@ -905,15 +1210,15 @@
         <v>-5.047244658319892</v>
       </c>
       <c r="F6" s="2">
-        <v>-3.898531300201868</v>
+        <v>-3.898531300201869</v>
       </c>
       <c r="G6" s="2">
         <v>-2.307308459846443</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>-3.388273760727137</v>
@@ -934,9 +1239,9 @@
         <v>-1.933056266862</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>-8.646858295086131</v>
@@ -957,9 +1262,9 @@
         <v>-6.354959956004122</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>-3.908484506897013</v>
@@ -980,388 +1285,414 @@
         <v>-502.3862268365551</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-8.694587451793977</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-5.001607901740306</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-8.589535088028967</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-5.039505066469673</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-6.637659783193147</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-2.684511089589303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-8.225725410743301</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-5.081176038899269</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-7.72387796345584</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-4.975578929445486</v>
+      </c>
+      <c r="F11" s="2">
+        <v>-6.054483016828362</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-2.805369201214518</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-7.140309121782519</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-4.53610735656565</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-7.180351718585901</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-4.55918392592814</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-3.185395955952746</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-2.15585503303971</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-7.237562585169607</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-4.542484230292279</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-7.169937667242639</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-4.548162638294063</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-3.207245727810262</v>
+      </c>
+      <c r="G13" s="2">
+        <v>-2.156356493014942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-7.342809358456657</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-4.536847897152252</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-7.274600286327456</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-4.555483763719328</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-3.20979691626329</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-2.148163658885881</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-2.406588519906642</v>
-      </c>
-      <c r="C13" s="2">
-        <v>-2.271839969276601</v>
-      </c>
-      <c r="D13" s="2">
-        <v>-12.38543644119261</v>
-      </c>
-      <c r="E13" s="2">
-        <v>-11.18164972792683</v>
-      </c>
-      <c r="F13" s="2">
-        <v>-12.63651954718999</v>
-      </c>
-      <c r="G13" s="2">
-        <v>-12.30792668984035</v>
-      </c>
-      <c r="H13" s="2">
-        <v>-15.20613322493774</v>
-      </c>
-      <c r="I13" s="2">
-        <v>-13.91747093993732</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
-        <v>-3.886903103568473</v>
-      </c>
-      <c r="C14" s="2">
-        <v>-2.442375061613417</v>
-      </c>
-      <c r="D14" s="2">
-        <v>-15.62547678250365</v>
-      </c>
-      <c r="E14" s="2">
-        <v>-12.91522449021419</v>
-      </c>
-      <c r="F14" s="2">
-        <v>-14.04437413313229</v>
-      </c>
-      <c r="G14" s="2">
-        <v>-12.8326259600118</v>
-      </c>
-      <c r="H14" s="2">
-        <v>-16.91786132864561</v>
-      </c>
-      <c r="I14" s="2">
-        <v>-14.96137893605646</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2">
-        <v>-1.519422232632343</v>
-      </c>
-      <c r="C15" s="2">
-        <v>-5.197980779624778</v>
-      </c>
-      <c r="D15" s="2">
-        <v>-8.169460968146819</v>
-      </c>
-      <c r="E15" s="2">
-        <v>-13.02043027910751</v>
-      </c>
-      <c r="F15" s="2">
-        <v>-11.1989295301357</v>
-      </c>
-      <c r="G15" s="2">
-        <v>-13.09912231080883</v>
-      </c>
-      <c r="H15" s="2">
-        <v>-13.80160108699204</v>
-      </c>
-      <c r="I15" s="2">
-        <v>-14.9433265266613</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2">
-        <v>-3.331051673610126</v>
-      </c>
-      <c r="C16" s="2">
-        <v>-2.684490485463122</v>
-      </c>
-      <c r="D16" s="2">
-        <v>-12.74419526460708</v>
-      </c>
-      <c r="E16" s="2">
-        <v>-11.5652301720163</v>
-      </c>
-      <c r="F16" s="2">
-        <v>-14.76857453305526</v>
-      </c>
-      <c r="G16" s="2">
-        <v>-13.24106316786271</v>
-      </c>
-      <c r="H16" s="2">
-        <v>-16.08738102852206</v>
-      </c>
-      <c r="I16" s="2">
-        <v>-14.29955186747264</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2">
-        <v>-2.353326823581802</v>
-      </c>
-      <c r="C17" s="2">
-        <v>-2.267334386802271</v>
-      </c>
-      <c r="D17" s="2">
-        <v>-11.35711174398738</v>
-      </c>
-      <c r="E17" s="2">
-        <v>-10.75493533527868</v>
-      </c>
-      <c r="F17" s="2">
-        <v>-12.28504958178243</v>
-      </c>
-      <c r="G17" s="2">
-        <v>-12.24800669286612</v>
-      </c>
-      <c r="H17" s="2">
-        <v>-14.29304155291099</v>
-      </c>
-      <c r="I17" s="2">
-        <v>-13.82318049248749</v>
+      <c r="C17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B18" s="2">
-        <v>-11.49228677303553</v>
+        <v>-2.406588519906642</v>
       </c>
       <c r="C18" s="2">
-        <v>-5.952711599023645</v>
+        <v>-2.271839969276601</v>
       </c>
       <c r="D18" s="2">
-        <v>-18.386072879347</v>
+        <v>-12.38543644119261</v>
       </c>
       <c r="E18" s="2">
-        <v>-18.21090727542332</v>
+        <v>-11.18164972792683</v>
       </c>
       <c r="F18" s="2">
-        <v>-17.31428358578747</v>
+        <v>-12.63651954718999</v>
       </c>
       <c r="G18" s="2">
-        <v>-17.68145187335185</v>
+        <v>-12.30792668984035</v>
       </c>
       <c r="H18" s="2">
-        <v>-18.32582658070821</v>
+        <v>-15.20613322493774</v>
       </c>
       <c r="I18" s="2">
-        <v>-18.11341865651037</v>
+        <v>-13.91747093993732</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2">
-        <v>-2.27054865275148</v>
+        <v>-3.886903103568473</v>
       </c>
       <c r="C19" s="2">
-        <v>-2.247765934191721</v>
+        <v>-2.442375061613417</v>
       </c>
       <c r="D19" s="2">
-        <v>-12.30822824251503</v>
+        <v>-15.62547678250365</v>
       </c>
       <c r="E19" s="2">
-        <v>-11.14457115230957</v>
+        <v>-12.91522449021419</v>
       </c>
       <c r="F19" s="2">
-        <v>-12.38491984390812</v>
+        <v>-14.04437413313229</v>
       </c>
       <c r="G19" s="2">
-        <v>-12.18134795111036</v>
+        <v>-12.8326259600118</v>
       </c>
       <c r="H19" s="2">
-        <v>-14.75879588234056</v>
+        <v>-16.91786132864561</v>
       </c>
       <c r="I19" s="2">
-        <v>-13.64782756674383</v>
+        <v>-14.96137893605646</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-1.519422232632343</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-5.197980779624778</v>
+      </c>
+      <c r="D20" s="2">
+        <v>-8.169460968146819</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-13.02043027910751</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-11.1989295301357</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-13.09912231080883</v>
+      </c>
+      <c r="H20" s="2">
+        <v>-13.80160108699204</v>
+      </c>
+      <c r="I20" s="2">
+        <v>-14.9433265266613</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="B21" s="2">
+        <v>-3.331051673610126</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-2.684490485463122</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-12.74419526460708</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-11.5652301720163</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-14.76857453305526</v>
+      </c>
+      <c r="G21" s="2">
+        <v>-13.24106316786271</v>
+      </c>
+      <c r="H21" s="2">
+        <v>-16.08738102852206</v>
+      </c>
+      <c r="I21" s="2">
+        <v>-14.29955186747264</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>34</v>
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2">
+        <v>-2.353326823581802</v>
+      </c>
+      <c r="C22" s="2">
+        <v>-2.267334386802271</v>
+      </c>
+      <c r="D22" s="2">
+        <v>-11.35711174398738</v>
+      </c>
+      <c r="E22" s="2">
+        <v>-10.75493533527868</v>
+      </c>
+      <c r="F22" s="2">
+        <v>-12.28504958178243</v>
+      </c>
+      <c r="G22" s="2">
+        <v>-12.24800669286612</v>
+      </c>
+      <c r="H22" s="2">
+        <v>-14.29304155291099</v>
+      </c>
+      <c r="I22" s="2">
+        <v>-13.82318049248749</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2">
-        <v>0.2913258510942334</v>
+        <v>-11.49228677303553</v>
       </c>
       <c r="C23" s="2">
-        <v>0.2735800862624911</v>
+        <v>-5.952711599023645</v>
       </c>
       <c r="D23" s="2">
-        <v>0.1613100713260165</v>
+        <v>-18.386072879347</v>
       </c>
       <c r="E23" s="2">
-        <v>0.1275350663961443</v>
+        <v>-18.21090727542332</v>
       </c>
       <c r="F23" s="2">
-        <v>0.343113704341413</v>
+        <v>-17.31428358578747</v>
       </c>
       <c r="G23" s="2">
-        <v>0.7206</v>
+        <v>-17.68145187335185</v>
       </c>
       <c r="H23" s="2">
-        <v>0.14935</v>
+        <v>-18.32582658070821</v>
       </c>
       <c r="I23" s="2">
-        <v>-61.09662317853844</v>
+        <v>-18.11341865651037</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2">
-        <v>0.5974197011936037</v>
+        <v>-2.27054865275148</v>
       </c>
       <c r="C24" s="2">
-        <v>0.3750530081503448</v>
+        <v>-2.247765934191721</v>
       </c>
       <c r="D24" s="2">
-        <v>0.6278324954628842</v>
+        <v>-12.30822824251503</v>
       </c>
       <c r="E24" s="2">
-        <v>0.3259333538935</v>
+        <v>-11.14457115230957</v>
       </c>
       <c r="F24" s="2">
-        <v>0.4832861331967759</v>
+        <v>-12.38491984390812</v>
       </c>
       <c r="G24" s="2">
-        <v>0.1446833333333333</v>
+        <v>-12.18134795111036</v>
       </c>
       <c r="H24" s="2">
-        <v>0.1197166666666667</v>
+        <v>-14.75879588234056</v>
       </c>
       <c r="I24" s="2">
-        <v>-0.09671273821676769</v>
+        <v>-13.64782756674383</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="2">
-        <v>0.2761666282714071</v>
+        <v>-4.061357846528513</v>
       </c>
       <c r="C25" s="2">
-        <v>0.06101217747468211</v>
+        <v>-2.476604854168365</v>
       </c>
       <c r="D25" s="2">
-        <v>0</v>
+        <v>-15.55403484057587</v>
       </c>
       <c r="E25" s="2">
-        <v>0.09819788058674699</v>
+        <v>-13.04840731373303</v>
       </c>
       <c r="F25" s="2">
-        <v>0.2706623868796735</v>
+        <v>-14.08953032693041</v>
       </c>
       <c r="G25" s="2">
-        <v>0.3749</v>
+        <v>-12.83823729463579</v>
       </c>
       <c r="H25" s="2">
-        <v>0.09156666666666667</v>
+        <v>-17.14158603737399</v>
       </c>
       <c r="I25" s="2">
-        <v>-5.255185386010393</v>
+        <v>-15.12959271964095</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B26" s="2">
-        <v>0.4262577542033918</v>
+        <v>-4.036251438079522</v>
       </c>
       <c r="C26" s="2">
-        <v>0.2899430368587291</v>
+        <v>-2.442525391425952</v>
       </c>
       <c r="D26" s="2">
-        <v>0.600426353460308</v>
+        <v>-15.39443511187351</v>
       </c>
       <c r="E26" s="2">
-        <v>0</v>
+        <v>-12.9447557929644</v>
+      </c>
+      <c r="F26" s="2">
+        <v>-14.00432031238853</v>
       </c>
       <c r="G26" s="2">
-        <v>0.07918333333333334</v>
+        <v>-12.80694477853251</v>
       </c>
       <c r="H26" s="2">
-        <v>0.07881666666666666</v>
+        <v>-16.98246106861659</v>
       </c>
       <c r="I26" s="2">
-        <v>-4.22744006074679</v>
+        <v>-15.00671687910291</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1369,80 +1700,468 @@
         <v>4</v>
       </c>
       <c r="B27" s="2">
-        <v>0.6301746613802992</v>
+        <v>-2.239472290887487</v>
       </c>
       <c r="C27" s="2">
-        <v>0.406640508967517</v>
+        <v>-3.472655054260665</v>
       </c>
       <c r="D27" s="2">
-        <v>0.07867086945101129</v>
+        <v>-12.92329475595288</v>
       </c>
       <c r="E27" s="2">
-        <v>0.4331591847169729</v>
+        <v>-15.5433506878912</v>
       </c>
       <c r="F27" s="2">
-        <v>0.4614386335762677</v>
+        <v>-16.39622224511263</v>
       </c>
       <c r="G27" s="2">
-        <v>0.7936666666666667</v>
+        <v>-15.52681145433409</v>
       </c>
       <c r="H27" s="2">
-        <v>0.7723166666666667</v>
+        <v>-17.81160777084134</v>
       </c>
       <c r="I27" s="2">
-        <v>-0.4426514751777253</v>
+        <v>-16.5626021792993</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
-        <v>0.1621415339290632</v>
+        <v>-2.754478097600628</v>
       </c>
       <c r="C28" s="2">
-        <v>0.05181635667822724</v>
+        <v>-2.984034863092522</v>
       </c>
       <c r="D28" s="2">
-        <v>0.1660303744910523</v>
+        <v>-14.58292537375742</v>
       </c>
       <c r="E28" s="2">
-        <v>0.09591554596683807</v>
+        <v>-14.57308187678406</v>
       </c>
       <c r="F28" s="2">
-        <v>0.1807969282858515</v>
+        <v>-16.90744617513097</v>
       </c>
       <c r="G28" s="2">
-        <v>0.3746833333333333</v>
+        <v>-15.39119342382116</v>
       </c>
       <c r="H28" s="2">
-        <v>0.1556333333333333</v>
+        <v>-18.01401453768404</v>
       </c>
       <c r="I28" s="2">
-        <v>-319605180.2536416</v>
+        <v>-16.5129410526756</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-2.316037136313853</v>
+      </c>
+      <c r="C29" s="2">
+        <v>-3.228358032393064</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-15.45403749790653</v>
+      </c>
+      <c r="E29" s="2">
+        <v>-15.66828186022075</v>
+      </c>
+      <c r="F29" s="2">
+        <v>-14.46271625971969</v>
+      </c>
+      <c r="G29" s="2">
+        <v>-15.29501357885881</v>
+      </c>
+      <c r="H29" s="2">
+        <v>-17.84564923427493</v>
+      </c>
+      <c r="I29" s="2">
+        <v>-17.93077212287599</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.2913258510942334</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.2735800862624911</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.1613100713260165</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.1275350663961443</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.343113704341413</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.7206</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.14935</v>
+      </c>
+      <c r="I33" s="2">
+        <v>-61.09662317853844</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.5974197011936037</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.3750530081503448</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.6278324954628842</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.3259333538935</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.4832861331967759</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.1446833333333333</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.1197166666666667</v>
+      </c>
+      <c r="I34" s="2">
+        <v>-0.09671273821676769</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.2761666282714071</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.06101217747468211</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.098197880586747</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.2706623868796735</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.3749</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.09156666666666667</v>
+      </c>
+      <c r="I35" s="2">
+        <v>-5.255185386010393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.4262577542033918</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.2899430368587291</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.600426353460308</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.07918333333333334</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.07881666666666666</v>
+      </c>
+      <c r="I36" s="2">
+        <v>-4.22744006074679</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.6301746613802992</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.406640508967517</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.07867086945101129</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.4331591847169729</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.4614386335762677</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.7936666666666667</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.7723166666666667</v>
+      </c>
+      <c r="I37" s="2">
+        <v>-0.4426514751777253</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.1621415339290632</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.05181635667822724</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.1660303744910523</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.09591554596683807</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.1807969282858515</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.3746833333333333</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.1556333333333333</v>
+      </c>
+      <c r="I38" s="2">
+        <v>-319605180.2536416</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.4361005523815438</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.1843732446981761</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.1656435958141934</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.2415233567590648</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.3533865528603071</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="2">
+        <v>-2.920691846838815</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.6145970526279479</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.3579274373895278</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.6427052748374273</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.3244070570381679</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.5311186394984133</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0.133</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.1297333333333333</v>
+      </c>
+      <c r="I40" s="2">
+        <v>-0.1097929715945471</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="2">
-        <v>0.4361005523815438</v>
-      </c>
-      <c r="C29" s="2">
-        <v>0.1843732446981761</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.1656435958141934</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0.2415233567590648</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0.3533865528603071</v>
-      </c>
-      <c r="I29" s="2">
-        <v>-2.920691846838815</v>
+      <c r="B41" s="2">
+        <v>0.5790016615031582</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.3241488295078014</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.6526329906958909</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.3229656644831733</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.5431617116568533</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.1913666666666667</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.1354</v>
+      </c>
+      <c r="I41" s="2">
+        <v>-0.08504466320868731</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.1359049022302793</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.1767806355571024</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.12765</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="2">
+        <v>-17.66777792521084</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.2945587776663055</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.08439879685146127</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.001139118630496176</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.1429418563648109</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.2718124006266754</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.1768500000000001</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.16315</v>
+      </c>
+      <c r="I43" s="2">
+        <v>-54.25491285245042</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.1856328338575214</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.1826265702357067</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.3352550179700383</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.4793166666666666</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.50475</v>
+      </c>
+      <c r="I44" s="2">
+        <v>-6.907813246789758</v>
       </c>
     </row>
   </sheetData>
@@ -1471,30 +2190,30 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1502,6 +2221,693 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
+        <v>-3.885928070248749</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-5.274841343089261</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-4.066210482168392</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-10.28741060403429</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-1.750592026788664</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-18.90481475924042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-9.162882145624636</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-5.066747087143494</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-8.653292980523496</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-5.086304003131836</v>
+      </c>
+      <c r="F4" s="2">
+        <v>-7.056121943207441</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-2.737148674403763</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-6.833268269910192</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-84.38058716048052</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-7.747477107037732</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-160.8991592658656</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-2.769543292809081</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-133.4629003196207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-6.777963983549516</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-4.931756213669246</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-7.080974443429973</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-5.047244658319892</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-3.898531300201868</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-2.307308459846443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-3.388273760727137</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-5.190145619137</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-3.820568826085621</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-3.724632603425154</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-1.654247003638594</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-1.933056266862</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-8.646858295086131</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-423.5732756751199</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-11.45854568625663</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-8.908475059016894</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-16.83063406863265</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-6.354959956004122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-3.908484506897013</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-7.334724098125236</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-4.08618993572303</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-8.532455255491085</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-1.785586399630908</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-502.3862268365551</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-2.406588519906642</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-2.271839969276601</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-12.38543644119261</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-11.18164972792683</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-12.63651954718999</v>
+      </c>
+      <c r="G13" s="2">
+        <v>-12.30792668984035</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-15.20613322493774</v>
+      </c>
+      <c r="I13" s="2">
+        <v>-13.91747093993732</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-3.886903103568473</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-2.442375061613417</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-15.62547678250365</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-12.91522449021419</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-14.04437413313229</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-12.8326259600118</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-16.91786132864561</v>
+      </c>
+      <c r="I14" s="2">
+        <v>-14.96137893605646</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>-1.519422232632343</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-5.197980779624778</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-8.169460968146819</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-13.02043027910751</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-11.1989295301357</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-13.09912231080883</v>
+      </c>
+      <c r="H15" s="2">
+        <v>-13.80160108699204</v>
+      </c>
+      <c r="I15" s="2">
+        <v>-14.9433265266613</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2">
+        <v>-3.331051673610126</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-2.684490485463122</v>
+      </c>
+      <c r="D16" s="2">
+        <v>-12.74419526460708</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-11.5652301720163</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-14.76857453305526</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-13.24106316786271</v>
+      </c>
+      <c r="H16" s="2">
+        <v>-16.08738102852206</v>
+      </c>
+      <c r="I16" s="2">
+        <v>-14.29955186747264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>-2.353326823581802</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-2.267334386802271</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-11.35711174398738</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-10.75493533527868</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-12.28504958178243</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-12.24800669286612</v>
+      </c>
+      <c r="H17" s="2">
+        <v>-14.29304155291099</v>
+      </c>
+      <c r="I17" s="2">
+        <v>-13.82318049248749</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2">
+        <v>-11.49228677303553</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-5.952711599023645</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-18.386072879347</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-18.21090727542332</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-17.31428358578747</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-17.68145187335185</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-18.32582658070821</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-18.11341865651037</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-2.27054865275148</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-2.247765934191721</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-12.30822824251503</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-11.14457115230957</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-12.38491984390812</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-12.18134795111036</v>
+      </c>
+      <c r="H19" s="2">
+        <v>-14.75879588234056</v>
+      </c>
+      <c r="I19" s="2">
+        <v>-13.64782756674383</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.2913258510942334</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.2735800862624911</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.1613100713260165</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.1275350663961443</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.343113704341413</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.7206</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.14935</v>
+      </c>
+      <c r="I23" s="2">
+        <v>-61.09662317853844</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.5974197011936037</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.3750530081503448</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.6278324954628842</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.3259333538935</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.4832861331967759</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.1446833333333333</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.1197166666666667</v>
+      </c>
+      <c r="I24" s="2">
+        <v>-0.09671273821676769</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.2761666282714071</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.06101217747468211</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.09819788058674699</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.2706623868796735</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.3749</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.09156666666666667</v>
+      </c>
+      <c r="I25" s="2">
+        <v>-5.255185386010393</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.4262577542033918</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.2899430368587291</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.600426353460308</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.07918333333333334</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.07881666666666666</v>
+      </c>
+      <c r="I26" s="2">
+        <v>-4.22744006074679</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.6301746613802992</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.406640508967517</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.07867086945101129</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.4331591847169729</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.4614386335762677</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.7936666666666667</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.7723166666666667</v>
+      </c>
+      <c r="I27" s="2">
+        <v>-0.4426514751777253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.1621415339290632</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.05181635667822724</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.1660303744910523</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.09591554596683807</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.1807969282858515</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.3746833333333333</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.1556333333333333</v>
+      </c>
+      <c r="I28" s="2">
+        <v>-319605180.2536416</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.4361005523815438</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.1843732446981761</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.1656435958141934</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.2415233567590648</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.3533865528603071</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="2">
+        <v>-2.920691846838815</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
         <v>-3.68</v>
       </c>
       <c r="C3" s="2">
@@ -1522,7 +2928,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>-4.33</v>
@@ -1545,7 +2951,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>-10.04</v>
@@ -1568,7 +2974,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>-9.81</v>
@@ -1591,7 +2997,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>-8.699999999999999</v>
@@ -1614,7 +3020,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>-2.86</v>
@@ -1637,7 +3043,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
         <v>-5.63</v>
@@ -1660,36 +3066,36 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1723,7 +3129,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>-2.28</v>
@@ -1752,7 +3158,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
         <v>-2.81</v>
@@ -1781,7 +3187,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2">
         <v>-8.109999999999999</v>
@@ -1810,7 +3216,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2">
         <v>-3.64</v>
@@ -1839,7 +3245,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2">
         <v>-2.31</v>
@@ -1868,7 +3274,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2">
         <v>-2.56</v>
@@ -1897,36 +3303,36 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1960,7 +3366,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2">
         <v>0.414</v>
@@ -1989,7 +3395,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2">
         <v>0.375</v>
@@ -2018,7 +3424,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B26" s="2">
         <v>0.235</v>
@@ -2047,7 +3453,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2">
         <v>0.4920000000000001</v>
@@ -2076,7 +3482,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2">
         <v>0.626</v>
@@ -2105,7 +3511,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" s="2">
         <v>0.601</v>

</xml_diff>

<commit_message>
New results and option to download datasets (#56)
* Bump version: 0.2.2.dev0 → 0.2.2.dev1

* Add command to download datasets without running sdgym

* Add progress bar to log

* cap pomegranate version

* Fix replace_existing argument

* Add latest results

* Update python versions on readme
</commit_message>
<xml_diff>
--- a/results/SDGym-Leaderboard.xlsx
+++ b/results/SDGym-Leaderboard.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Number of wins per version" sheetId="1" r:id="rId1"/>
-    <sheet name="0.2.2.dev0" sheetId="2" r:id="rId2"/>
+    <sheet name="0.2.2" sheetId="2" r:id="rId2"/>
     <sheet name="0.2.1" sheetId="3" r:id="rId3"/>
     <sheet name="0.2.0" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="42">
   <si>
     <t>CLBNSynthesizer</t>
   </si>
@@ -64,7 +64,7 @@
     <t>Synthesizer</t>
   </si>
   <si>
-    <t>0.2.2.dev0</t>
+    <t>0.2.2</t>
   </si>
   <si>
     <t>0.2.1</t>
@@ -506,7 +506,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" style="2" customWidth="1"/>
   </cols>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>12</v>
@@ -1035,7 +1035,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="2">
         <v>5</v>
@@ -1129,275 +1129,275 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>-3.885928070248749</v>
+        <v>-3.883163747038106</v>
       </c>
       <c r="C3" s="2">
-        <v>-5.274841343089261</v>
+        <v>-9.202143870182695</v>
       </c>
       <c r="D3" s="2">
-        <v>-4.066210482168392</v>
+        <v>-4.008392448737879</v>
       </c>
       <c r="E3" s="2">
-        <v>-10.28741060403429</v>
+        <v>-7.432801259089946</v>
       </c>
       <c r="F3" s="2">
-        <v>-1.750592026788664</v>
+        <v>-1.765073421953277</v>
       </c>
       <c r="G3" s="2">
-        <v>-18.90481475924042</v>
+        <v>-47.15793612179723</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>-9.162882145624636</v>
+        <v>-8.760635266641627</v>
       </c>
       <c r="C4" s="2">
-        <v>-5.066747087143494</v>
+        <v>-5.062972106881769</v>
       </c>
       <c r="D4" s="2">
-        <v>-8.653292980523496</v>
+        <v>-8.309750284710571</v>
       </c>
       <c r="E4" s="2">
-        <v>-5.086304003131836</v>
+        <v>-5.048309525940072</v>
       </c>
       <c r="F4" s="2">
-        <v>-7.056121943207441</v>
+        <v>-6.591323889622508</v>
       </c>
       <c r="G4" s="2">
-        <v>-2.737148674403763</v>
+        <v>-2.665281471285607</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>-6.833268269910192</v>
+        <v>-8.918386257639886</v>
       </c>
       <c r="C5" s="2">
-        <v>-84.38058716048052</v>
+        <v>-5.088557286899332</v>
       </c>
       <c r="D5" s="2">
-        <v>-7.747477107037732</v>
+        <v>-8.323578368237701</v>
       </c>
       <c r="E5" s="2">
-        <v>-160.8991592658656</v>
+        <v>-5.02729290814621</v>
       </c>
       <c r="F5" s="2">
-        <v>-2.769543292809081</v>
+        <v>-7.130586043802099</v>
       </c>
       <c r="G5" s="2">
-        <v>-133.4629003196207</v>
+        <v>-2.704076182028625</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>-6.777963983549516</v>
+        <v>-8.190169410566059</v>
       </c>
       <c r="C6" s="2">
-        <v>-4.931756213669246</v>
+        <v>-5.141363329314994</v>
       </c>
       <c r="D6" s="2">
-        <v>-7.080974443429973</v>
+        <v>-8.162766717527328</v>
       </c>
       <c r="E6" s="2">
-        <v>-5.047244658319892</v>
+        <v>-5.0054700047586</v>
       </c>
       <c r="F6" s="2">
-        <v>-3.898531300201869</v>
+        <v>-6.20616566233844</v>
       </c>
       <c r="G6" s="2">
-        <v>-2.307308459846443</v>
+        <v>-2.80004284451614</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>-3.388273760727137</v>
+        <v>-7.235399290973477</v>
       </c>
       <c r="C7" s="2">
-        <v>-5.190145619137</v>
+        <v>-4.511048877959109</v>
       </c>
       <c r="D7" s="2">
-        <v>-3.820568826085621</v>
+        <v>-7.164373783184903</v>
       </c>
       <c r="E7" s="2">
-        <v>-3.724632603425154</v>
+        <v>-4.543400391678849</v>
       </c>
       <c r="F7" s="2">
-        <v>-1.654247003638594</v>
+        <v>-3.196911857539349</v>
       </c>
       <c r="G7" s="2">
-        <v>-1.933056266862</v>
+        <v>-2.150929600900062</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>-8.646858295086131</v>
+        <v>-7.344125756946834</v>
       </c>
       <c r="C8" s="2">
-        <v>-423.5732756751199</v>
+        <v>-4.565754467063921</v>
       </c>
       <c r="D8" s="2">
-        <v>-11.45854568625663</v>
+        <v>-7.144525105266569</v>
       </c>
       <c r="E8" s="2">
-        <v>-8.908475059016894</v>
+        <v>-4.554080028497022</v>
       </c>
       <c r="F8" s="2">
-        <v>-16.83063406863265</v>
+        <v>-3.17900097117842</v>
       </c>
       <c r="G8" s="2">
-        <v>-6.354959956004122</v>
+        <v>-2.154148419236831</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>-3.908484506897013</v>
+        <v>-7.268047175966656</v>
       </c>
       <c r="C9" s="2">
-        <v>-7.334724098125236</v>
+        <v>-4.514381130130833</v>
       </c>
       <c r="D9" s="2">
-        <v>-4.08618993572303</v>
+        <v>-7.192245751193527</v>
       </c>
       <c r="E9" s="2">
-        <v>-8.532455255491085</v>
+        <v>-4.550714962639452</v>
       </c>
       <c r="F9" s="2">
-        <v>-1.785586399630908</v>
+        <v>-3.207624381824364</v>
       </c>
       <c r="G9" s="2">
-        <v>-502.3862268365551</v>
+        <v>-2.154493398585112</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>-8.694587451793977</v>
+        <v>-5.829463312159628</v>
       </c>
       <c r="C10" s="2">
-        <v>-5.001607901740306</v>
+        <v>-90.34196023047687</v>
       </c>
       <c r="D10" s="2">
-        <v>-8.589535088028967</v>
+        <v>-7.37063381135388</v>
       </c>
       <c r="E10" s="2">
-        <v>-5.039505066469673</v>
+        <v>-141.4065766962444</v>
       </c>
       <c r="F10" s="2">
-        <v>-6.637659783193147</v>
+        <v>-2.779566471702924</v>
       </c>
       <c r="G10" s="2">
-        <v>-2.684511089589303</v>
+        <v>-149.766976540331</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>-8.225725410743301</v>
+        <v>-3.994404488185729</v>
       </c>
       <c r="C11" s="2">
-        <v>-5.081176038899269</v>
+        <v>-8.308435277882692</v>
       </c>
       <c r="D11" s="2">
-        <v>-7.72387796345584</v>
+        <v>-4.07166054347988</v>
       </c>
       <c r="E11" s="2">
-        <v>-4.975578929445486</v>
-      </c>
-      <c r="F11" s="2">
-        <v>-6.054483016828362</v>
-      </c>
-      <c r="G11" s="2">
-        <v>-2.805369201214518</v>
+        <v>-7.121354377721727</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>-7.140309121782519</v>
+        <v>-3.26779099008614</v>
       </c>
       <c r="C12" s="2">
-        <v>-4.53610735656565</v>
+        <v>-5.657797017261816</v>
       </c>
       <c r="D12" s="2">
-        <v>-7.180351718585901</v>
+        <v>-3.867225435725924</v>
       </c>
       <c r="E12" s="2">
-        <v>-4.55918392592814</v>
+        <v>-3.70828249773228</v>
       </c>
       <c r="F12" s="2">
-        <v>-3.185395955952746</v>
+        <v>-1.579841230313827</v>
       </c>
       <c r="G12" s="2">
-        <v>-2.15585503303971</v>
+        <v>-1.939996795543686</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2">
-        <v>-7.237562585169607</v>
+        <v>-6.992157289486403</v>
       </c>
       <c r="C13" s="2">
-        <v>-4.542484230292279</v>
+        <v>-5.330743495969986</v>
       </c>
       <c r="D13" s="2">
-        <v>-7.169937667242639</v>
+        <v>-6.998887628745389</v>
       </c>
       <c r="E13" s="2">
-        <v>-4.548162638294063</v>
+        <v>-4.829217865606727</v>
       </c>
       <c r="F13" s="2">
-        <v>-3.207245727810262</v>
+        <v>-4.740190371698341</v>
       </c>
       <c r="G13" s="2">
-        <v>-2.156356493014942</v>
+        <v>-2.533675431723123</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2">
-        <v>-7.342809358456657</v>
+        <v>-8.646858295086131</v>
       </c>
       <c r="C14" s="2">
-        <v>-4.536847897152252</v>
+        <v>-423.5732756751199</v>
       </c>
       <c r="D14" s="2">
-        <v>-7.274600286327456</v>
+        <v>-11.45854568625663</v>
       </c>
       <c r="E14" s="2">
-        <v>-4.555483763719328</v>
+        <v>-8.908475059016894</v>
       </c>
       <c r="F14" s="2">
-        <v>-3.20979691626329</v>
+        <v>-16.83063406863265</v>
       </c>
       <c r="G14" s="2">
-        <v>-2.148163658885881</v>
+        <v>-6.354959956004122</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1439,347 +1439,347 @@
         <v>0</v>
       </c>
       <c r="B18" s="2">
-        <v>-2.406588519906642</v>
+        <v>-2.402547106844601</v>
       </c>
       <c r="C18" s="2">
-        <v>-2.271839969276601</v>
+        <v>-2.273803539803658</v>
       </c>
       <c r="D18" s="2">
-        <v>-12.38543644119261</v>
+        <v>-12.45884777673006</v>
       </c>
       <c r="E18" s="2">
-        <v>-11.18164972792683</v>
+        <v>-11.18780460800946</v>
       </c>
       <c r="F18" s="2">
-        <v>-12.63651954718999</v>
+        <v>-12.6258566343313</v>
       </c>
       <c r="G18" s="2">
-        <v>-12.30792668984035</v>
+        <v>-12.30673698777013</v>
       </c>
       <c r="H18" s="2">
-        <v>-15.20613322493774</v>
+        <v>-15.16680341865399</v>
       </c>
       <c r="I18" s="2">
-        <v>-13.91747093993732</v>
+        <v>-13.91763423318691</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="2">
-        <v>-3.886903103568473</v>
+        <v>-4.187959782867199</v>
       </c>
       <c r="C19" s="2">
-        <v>-2.442375061613417</v>
+        <v>-2.455443886356906</v>
       </c>
       <c r="D19" s="2">
-        <v>-15.62547678250365</v>
+        <v>-15.88204061145396</v>
       </c>
       <c r="E19" s="2">
-        <v>-12.91522449021419</v>
+        <v>-13.09755888297466</v>
       </c>
       <c r="F19" s="2">
-        <v>-14.04437413313229</v>
+        <v>-14.35352058946426</v>
       </c>
       <c r="G19" s="2">
-        <v>-12.8326259600118</v>
+        <v>-12.84035746938658</v>
       </c>
       <c r="H19" s="2">
-        <v>-16.91786132864561</v>
+        <v>-17.02601096082736</v>
       </c>
       <c r="I19" s="2">
-        <v>-14.96137893605646</v>
+        <v>-14.97252075714458</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2">
-        <v>-1.519422232632343</v>
+        <v>-2.693441309893506</v>
       </c>
       <c r="C20" s="2">
-        <v>-5.197980779624778</v>
+        <v>-2.311809822000515</v>
       </c>
       <c r="D20" s="2">
-        <v>-8.169460968146819</v>
+        <v>-15.22044773715002</v>
       </c>
       <c r="E20" s="2">
-        <v>-13.02043027910751</v>
+        <v>-12.92800957916587</v>
       </c>
       <c r="F20" s="2">
-        <v>-11.1989295301357</v>
+        <v>-13.80822033524588</v>
       </c>
       <c r="G20" s="2">
-        <v>-13.09912231080883</v>
+        <v>-12.81246637757621</v>
       </c>
       <c r="H20" s="2">
-        <v>-13.80160108699204</v>
+        <v>-16.59828761832473</v>
       </c>
       <c r="I20" s="2">
-        <v>-14.9433265266613</v>
+        <v>-14.8406335450323</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2">
-        <v>-3.331051673610126</v>
+        <v>-3.956070743305794</v>
       </c>
       <c r="C21" s="2">
-        <v>-2.684490485463122</v>
+        <v>-2.404006665030712</v>
       </c>
       <c r="D21" s="2">
-        <v>-12.74419526460708</v>
+        <v>-15.68813093535282</v>
       </c>
       <c r="E21" s="2">
-        <v>-11.5652301720163</v>
+        <v>-13.05285050660692</v>
       </c>
       <c r="F21" s="2">
-        <v>-14.76857453305526</v>
+        <v>-14.24718214843184</v>
       </c>
       <c r="G21" s="2">
-        <v>-13.24106316786271</v>
+        <v>-12.91652234165256</v>
       </c>
       <c r="H21" s="2">
-        <v>-16.08738102852206</v>
+        <v>-16.95847961467858</v>
       </c>
       <c r="I21" s="2">
-        <v>-14.29955186747264</v>
+        <v>-14.95766967699486</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2">
-        <v>-2.353326823581802</v>
+        <v>-2.248123258940747</v>
       </c>
       <c r="C22" s="2">
-        <v>-2.267334386802271</v>
+        <v>-3.612160533557288</v>
       </c>
       <c r="D22" s="2">
-        <v>-11.35711174398738</v>
+        <v>-12.90637895726414</v>
       </c>
       <c r="E22" s="2">
-        <v>-10.75493533527868</v>
+        <v>-15.57488203968424</v>
       </c>
       <c r="F22" s="2">
-        <v>-12.28504958178243</v>
+        <v>-16.40190575405644</v>
       </c>
       <c r="G22" s="2">
-        <v>-12.24800669286612</v>
+        <v>-15.54613676137945</v>
       </c>
       <c r="H22" s="2">
-        <v>-14.29304155291099</v>
+        <v>-17.83789065848317</v>
       </c>
       <c r="I22" s="2">
-        <v>-13.82318049248749</v>
+        <v>-16.57839994262226</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2">
-        <v>-11.49228677303553</v>
+        <v>-2.829653149586667</v>
       </c>
       <c r="C23" s="2">
-        <v>-5.952711599023645</v>
+        <v>-3.108912027229053</v>
       </c>
       <c r="D23" s="2">
-        <v>-18.386072879347</v>
+        <v>-14.52154307829453</v>
       </c>
       <c r="E23" s="2">
-        <v>-18.21090727542332</v>
+        <v>-14.56506397204311</v>
       </c>
       <c r="F23" s="2">
-        <v>-17.31428358578747</v>
+        <v>-16.89512904855699</v>
       </c>
       <c r="G23" s="2">
-        <v>-17.68145187335185</v>
+        <v>-15.40528408057893</v>
       </c>
       <c r="H23" s="2">
-        <v>-18.32582658070821</v>
+        <v>-18.02829248021571</v>
       </c>
       <c r="I23" s="2">
-        <v>-18.11341865651037</v>
+        <v>-16.51737013559032</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2">
-        <v>-2.27054865275148</v>
+        <v>-2.313891114432964</v>
       </c>
       <c r="C24" s="2">
-        <v>-2.247765934191721</v>
+        <v>-3.226644224332941</v>
       </c>
       <c r="D24" s="2">
-        <v>-12.30822824251503</v>
+        <v>-15.47606426425534</v>
       </c>
       <c r="E24" s="2">
-        <v>-11.14457115230957</v>
+        <v>-15.66633600334285</v>
       </c>
       <c r="F24" s="2">
-        <v>-12.38491984390812</v>
+        <v>-14.48281156414748</v>
       </c>
       <c r="G24" s="2">
-        <v>-12.18134795111036</v>
+        <v>-15.30611821407162</v>
       </c>
       <c r="H24" s="2">
-        <v>-14.75879588234056</v>
+        <v>-17.8436989494514</v>
       </c>
       <c r="I24" s="2">
-        <v>-13.64782756674383</v>
+        <v>-17.90746413901408</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2">
-        <v>-4.061357846528513</v>
+        <v>-1.574215242177617</v>
       </c>
       <c r="C25" s="2">
-        <v>-2.476604854168365</v>
+        <v>-5.965560306771161</v>
       </c>
       <c r="D25" s="2">
-        <v>-15.55403484057587</v>
+        <v>-7.838956449109022</v>
       </c>
       <c r="E25" s="2">
-        <v>-13.04840731373303</v>
+        <v>-13.25515563536335</v>
       </c>
       <c r="F25" s="2">
-        <v>-14.08953032693041</v>
+        <v>-11.11251913336074</v>
       </c>
       <c r="G25" s="2">
-        <v>-12.83823729463579</v>
+        <v>-12.98697357352015</v>
       </c>
       <c r="H25" s="2">
-        <v>-17.14158603737399</v>
+        <v>-13.88384850736239</v>
       </c>
       <c r="I25" s="2">
-        <v>-15.12959271964095</v>
+        <v>-15.07767369634699</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2">
-        <v>-4.036251438079522</v>
+        <v>-2.293589593953942</v>
       </c>
       <c r="C26" s="2">
-        <v>-2.442525391425952</v>
+        <v>-2.244695092983717</v>
       </c>
       <c r="D26" s="2">
-        <v>-15.39443511187351</v>
+        <v>-12.15366085843059</v>
       </c>
       <c r="E26" s="2">
-        <v>-12.9447557929644</v>
+        <v>-11.1396058639398</v>
       </c>
       <c r="F26" s="2">
-        <v>-14.00432031238853</v>
+        <v>-12.3600543136947</v>
       </c>
       <c r="G26" s="2">
-        <v>-12.80694477853251</v>
+        <v>-12.18768901035606</v>
       </c>
       <c r="H26" s="2">
-        <v>-16.98246106861659</v>
+        <v>-14.70178148834679</v>
       </c>
       <c r="I26" s="2">
-        <v>-15.00671687910291</v>
+        <v>-13.63706238463702</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2">
-        <v>-2.239472290887487</v>
+        <v>-2.293483332856178</v>
       </c>
       <c r="C27" s="2">
-        <v>-3.472655054260665</v>
+        <v>-2.266323182185946</v>
       </c>
       <c r="D27" s="2">
-        <v>-12.92329475595288</v>
+        <v>-11.44179159778551</v>
       </c>
       <c r="E27" s="2">
-        <v>-15.5433506878912</v>
+        <v>-10.76053628843016</v>
       </c>
       <c r="F27" s="2">
-        <v>-16.39622224511263</v>
+        <v>-12.45935730548618</v>
       </c>
       <c r="G27" s="2">
-        <v>-15.52681145433409</v>
+        <v>-12.29596499591153</v>
       </c>
       <c r="H27" s="2">
-        <v>-17.81160777084134</v>
+        <v>-14.29506264694043</v>
       </c>
       <c r="I27" s="2">
-        <v>-16.5626021792993</v>
+        <v>-14.23669937305969</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2">
-        <v>-2.754478097600628</v>
+        <v>-3.400134844931123</v>
       </c>
       <c r="C28" s="2">
-        <v>-2.984034863092522</v>
+        <v>-2.72081458032878</v>
       </c>
       <c r="D28" s="2">
-        <v>-14.58292537375742</v>
+        <v>-12.68884366958686</v>
       </c>
       <c r="E28" s="2">
-        <v>-14.57308187678406</v>
+        <v>-11.54235495350539</v>
       </c>
       <c r="F28" s="2">
-        <v>-16.90744617513097</v>
+        <v>-15.01679035454709</v>
       </c>
       <c r="G28" s="2">
-        <v>-15.39119342382116</v>
+        <v>-13.39289872916671</v>
       </c>
       <c r="H28" s="2">
-        <v>-18.01401453768404</v>
+        <v>-16.17812729368509</v>
       </c>
       <c r="I28" s="2">
-        <v>-16.5129410526756</v>
+        <v>-14.31876278557394</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2">
-        <v>-2.316037136313853</v>
+        <v>-11.49228677303553</v>
       </c>
       <c r="C29" s="2">
-        <v>-3.228358032393064</v>
+        <v>-5.952711599023645</v>
       </c>
       <c r="D29" s="2">
-        <v>-15.45403749790653</v>
+        <v>-18.386072879347</v>
       </c>
       <c r="E29" s="2">
-        <v>-15.66828186022075</v>
+        <v>-18.21090727542332</v>
       </c>
       <c r="F29" s="2">
-        <v>-14.46271625971969</v>
+        <v>-17.31428358578747</v>
       </c>
       <c r="G29" s="2">
-        <v>-15.29501357885881</v>
+        <v>-17.68145187335185</v>
       </c>
       <c r="H29" s="2">
-        <v>-17.84564923427493</v>
+        <v>-18.32582658070821</v>
       </c>
       <c r="I29" s="2">
-        <v>-17.93077212287599</v>
+        <v>-18.11341865651037</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1821,347 +1821,347 @@
         <v>0</v>
       </c>
       <c r="B33" s="2">
-        <v>0.2913258510942334</v>
+        <v>0.3050826982257354</v>
       </c>
       <c r="C33" s="2">
-        <v>0.2735800862624911</v>
+        <v>0.2857144781537949</v>
       </c>
       <c r="D33" s="2">
-        <v>0.1613100713260165</v>
+        <v>0.4406426400347374</v>
       </c>
       <c r="E33" s="2">
-        <v>0.1275350663961443</v>
+        <v>0.3296363311749395</v>
       </c>
       <c r="F33" s="2">
-        <v>0.343113704341413</v>
+        <v>0.3852430721992819</v>
       </c>
       <c r="G33" s="2">
-        <v>0.7206</v>
+        <v>0.7201</v>
       </c>
       <c r="H33" s="2">
-        <v>0.14935</v>
+        <v>0.16315</v>
       </c>
       <c r="I33" s="2">
-        <v>-61.09662317853844</v>
+        <v>-6.471832491208214</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" s="2">
-        <v>0.5974197011936037</v>
+        <v>0.6081788438500754</v>
       </c>
       <c r="C34" s="2">
-        <v>0.3750530081503448</v>
+        <v>0.3288147553792268</v>
       </c>
       <c r="D34" s="2">
-        <v>0.6278324954628842</v>
+        <v>0.6597709617487143</v>
       </c>
       <c r="E34" s="2">
-        <v>0.3259333538935</v>
+        <v>0.3166202007167158</v>
       </c>
       <c r="F34" s="2">
-        <v>0.4832861331967759</v>
+        <v>0.5405981706770625</v>
       </c>
       <c r="G34" s="2">
-        <v>0.1446833333333333</v>
+        <v>0.1223166666666667</v>
       </c>
       <c r="H34" s="2">
-        <v>0.1197166666666667</v>
+        <v>0.13775</v>
       </c>
       <c r="I34" s="2">
-        <v>-0.09671273821676769</v>
+        <v>-0.06959804793361481</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B35" s="2">
-        <v>0.2761666282714071</v>
+        <v>0.6024072900154367</v>
       </c>
       <c r="C35" s="2">
-        <v>0.06101217747468211</v>
+        <v>0.3788430324392779</v>
       </c>
       <c r="D35" s="2">
-        <v>0</v>
+        <v>0.5233384030145461</v>
       </c>
       <c r="E35" s="2">
-        <v>0.098197880586747</v>
+        <v>0.3297511068939431</v>
       </c>
       <c r="F35" s="2">
-        <v>0.2706623868796735</v>
+        <v>0.510841888605536</v>
       </c>
       <c r="G35" s="2">
-        <v>0.3749</v>
+        <v>0.14675</v>
       </c>
       <c r="H35" s="2">
-        <v>0.09156666666666667</v>
+        <v>0.1124666666666667</v>
       </c>
       <c r="I35" s="2">
-        <v>-5.255185386010393</v>
+        <v>-0.512953590553904</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B36" s="2">
-        <v>0.4262577542033918</v>
+        <v>0.6066379960376017</v>
       </c>
       <c r="C36" s="2">
-        <v>0.2899430368587291</v>
+        <v>0.3876630696086705</v>
       </c>
       <c r="D36" s="2">
-        <v>0.600426353460308</v>
+        <v>0.7174486803519062</v>
       </c>
       <c r="E36" s="2">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>12</v>
+        <v>0.3269410746094711</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.5165884828741659</v>
       </c>
       <c r="G36" s="2">
-        <v>0.07918333333333334</v>
+        <v>0.1590166666666667</v>
       </c>
       <c r="H36" s="2">
-        <v>0.07881666666666666</v>
+        <v>0.1492333333333333</v>
       </c>
       <c r="I36" s="2">
-        <v>-4.22744006074679</v>
+        <v>-0.05557033970743599</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0.6301746613802992</v>
+        <v>4</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C37" s="2">
-        <v>0.406640508967517</v>
+        <v>0</v>
       </c>
       <c r="D37" s="2">
-        <v>0.07867086945101129</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2">
-        <v>0.4331591847169729</v>
+        <v>0.1400198934375747</v>
       </c>
       <c r="F37" s="2">
-        <v>0.4614386335762677</v>
+        <v>0.176792311617512</v>
       </c>
       <c r="G37" s="2">
-        <v>0.7936666666666667</v>
-      </c>
-      <c r="H37" s="2">
-        <v>0.7723166666666667</v>
+        <v>0.1247666666666667</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I37" s="2">
-        <v>-0.4426514751777253</v>
+        <v>-5.029096289312759</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2">
-        <v>0.1621415339290632</v>
+        <v>0.2577479430105856</v>
       </c>
       <c r="C38" s="2">
-        <v>0.05181635667822724</v>
+        <v>0.05352759896916238</v>
       </c>
       <c r="D38" s="2">
-        <v>0.1660303744910523</v>
+        <v>0.01034419523179082</v>
       </c>
       <c r="E38" s="2">
-        <v>0.09591554596683807</v>
+        <v>0.138725688557952</v>
       </c>
       <c r="F38" s="2">
-        <v>0.1807969282858515</v>
+        <v>0.256446581500444</v>
       </c>
       <c r="G38" s="2">
-        <v>0.3746833333333333</v>
+        <v>0.1684</v>
       </c>
       <c r="H38" s="2">
-        <v>0.1556333333333333</v>
+        <v>0.1760166666666667</v>
       </c>
       <c r="I38" s="2">
-        <v>-319605180.2536416</v>
+        <v>-8.655143355730615</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B39" s="2">
-        <v>0.4361005523815438</v>
+        <v>0.1980418387489495</v>
       </c>
       <c r="C39" s="2">
-        <v>0.1843732446981761</v>
+        <v>0.1328295808998257</v>
       </c>
       <c r="D39" s="2">
-        <v>0.1656435958141934</v>
+        <v>0</v>
       </c>
       <c r="E39" s="2">
-        <v>0.2415233567590648</v>
+        <v>0.1822623775766875</v>
       </c>
       <c r="F39" s="2">
-        <v>0.3533865528603071</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>12</v>
+        <v>0.3311059480827125</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.4853833333333333</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.4930666666666667</v>
       </c>
       <c r="I39" s="2">
-        <v>-2.920691846838815</v>
+        <v>-36.94309380139293</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B40" s="2">
-        <v>0.6145970526279479</v>
+        <v>0.2433453961687154</v>
       </c>
       <c r="C40" s="2">
-        <v>0.3579274373895278</v>
+        <v>0.1364706642749178</v>
       </c>
       <c r="D40" s="2">
-        <v>0.6427052748374273</v>
+        <v>0.02440296578361119</v>
       </c>
       <c r="E40" s="2">
-        <v>0.3244070570381679</v>
+        <v>0.09113087846316033</v>
       </c>
       <c r="F40" s="2">
-        <v>0.5311186394984133</v>
+        <v>0.2745755068455984</v>
       </c>
       <c r="G40" s="2">
-        <v>0.133</v>
+        <v>0.3766666666666666</v>
       </c>
       <c r="H40" s="2">
-        <v>0.1297333333333333</v>
+        <v>0.10455</v>
       </c>
       <c r="I40" s="2">
-        <v>-0.1097929715945471</v>
+        <v>-5.601461962200701</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B41" s="2">
-        <v>0.5790016615031582</v>
+        <v>0.4287315085247321</v>
       </c>
       <c r="C41" s="2">
-        <v>0.3241488295078014</v>
+        <v>0.2447193365498767</v>
       </c>
       <c r="D41" s="2">
-        <v>0.6526329906958909</v>
+        <v>0.01097303374034364</v>
       </c>
       <c r="E41" s="2">
-        <v>0.3229656644831733</v>
+        <v>0.2147134516253093</v>
       </c>
       <c r="F41" s="2">
-        <v>0.5431617116568533</v>
-      </c>
-      <c r="G41" s="2">
-        <v>0.1913666666666667</v>
-      </c>
-      <c r="H41" s="2">
-        <v>0.1354</v>
-      </c>
-      <c r="I41" s="2">
-        <v>-0.08504466320868731</v>
+        <v>0.3826371889074425</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.6188661735370505</v>
       </c>
       <c r="C42" s="2">
-        <v>0</v>
+        <v>0.3823206825483227</v>
       </c>
       <c r="D42" s="2">
         <v>0</v>
       </c>
       <c r="E42" s="2">
-        <v>0.1359049022302793</v>
+        <v>0.4564466571953651</v>
       </c>
       <c r="F42" s="2">
-        <v>0.1767806355571024</v>
+        <v>0.4327523846094156</v>
       </c>
       <c r="G42" s="2">
-        <v>0.12765</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>12</v>
+        <v>0.7791166666666668</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.7692333333333333</v>
       </c>
       <c r="I42" s="2">
-        <v>-17.66777792521084</v>
+        <v>-0.2447827835562018</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B43" s="2">
-        <v>0.2945587776663055</v>
+        <v>0.3525372097168393</v>
       </c>
       <c r="C43" s="2">
-        <v>0.08439879685146127</v>
+        <v>0.2721201391853403</v>
       </c>
       <c r="D43" s="2">
-        <v>0.001139118630496176</v>
+        <v>0.2702991193680926</v>
       </c>
       <c r="E43" s="2">
-        <v>0.1429418563648109</v>
-      </c>
-      <c r="F43" s="2">
-        <v>0.2718124006266754</v>
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G43" s="2">
-        <v>0.1768500000000001</v>
+        <v>0.0872</v>
       </c>
       <c r="H43" s="2">
-        <v>0.16315</v>
+        <v>0.08291666666666668</v>
       </c>
       <c r="I43" s="2">
-        <v>-54.25491285245042</v>
+        <v>-5.820766780081367</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B44" s="2">
-        <v>0.1856328338575214</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>12</v>
+        <v>0.1621415339290632</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.05181635667822724</v>
       </c>
       <c r="D44" s="2">
-        <v>0</v>
+        <v>0.1660303744910523</v>
       </c>
       <c r="E44" s="2">
-        <v>0.1826265702357067</v>
+        <v>0.09591554596683807</v>
       </c>
       <c r="F44" s="2">
-        <v>0.3352550179700383</v>
+        <v>0.1807969282858515</v>
       </c>
       <c r="G44" s="2">
-        <v>0.4793166666666666</v>
+        <v>0.3746833333333333</v>
       </c>
       <c r="H44" s="2">
-        <v>0.50475</v>
+        <v>0.1556333333333333</v>
       </c>
       <c r="I44" s="2">
-        <v>-6.907813246789758</v>
+        <v>-319605180.2536416</v>
       </c>
     </row>
   </sheetData>
@@ -2287,25 +2287,25 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>-6.777963983549516</v>
+        <v>-3.908484506897013</v>
       </c>
       <c r="C6" s="2">
-        <v>-4.931756213669246</v>
+        <v>-7.334724098125236</v>
       </c>
       <c r="D6" s="2">
-        <v>-7.080974443429973</v>
+        <v>-4.08618993572303</v>
       </c>
       <c r="E6" s="2">
-        <v>-5.047244658319892</v>
+        <v>-8.532455255491085</v>
       </c>
       <c r="F6" s="2">
-        <v>-3.898531300201868</v>
+        <v>-1.785586399630908</v>
       </c>
       <c r="G6" s="2">
-        <v>-2.307308459846443</v>
+        <v>-502.3862268365551</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2333,48 +2333,48 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>-8.646858295086131</v>
+        <v>-6.777963983549516</v>
       </c>
       <c r="C8" s="2">
-        <v>-423.5732756751199</v>
+        <v>-4.931756213669246</v>
       </c>
       <c r="D8" s="2">
-        <v>-11.45854568625663</v>
+        <v>-7.080974443429973</v>
       </c>
       <c r="E8" s="2">
-        <v>-8.908475059016894</v>
+        <v>-5.047244658319892</v>
       </c>
       <c r="F8" s="2">
-        <v>-16.83063406863265</v>
+        <v>-3.898531300201868</v>
       </c>
       <c r="G8" s="2">
-        <v>-6.354959956004122</v>
+        <v>-2.307308459846443</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>-3.908484506897013</v>
+        <v>-8.646858295086131</v>
       </c>
       <c r="C9" s="2">
-        <v>-7.334724098125236</v>
+        <v>-423.5732756751199</v>
       </c>
       <c r="D9" s="2">
-        <v>-4.08618993572303</v>
+        <v>-11.45854568625663</v>
       </c>
       <c r="E9" s="2">
-        <v>-8.532455255491085</v>
+        <v>-8.908475059016894</v>
       </c>
       <c r="F9" s="2">
-        <v>-1.785586399630908</v>
+        <v>-16.83063406863265</v>
       </c>
       <c r="G9" s="2">
-        <v>-502.3862268365551</v>
+        <v>-6.354959956004122</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2500,31 +2500,31 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
-        <v>-3.331051673610126</v>
+        <v>-2.27054865275148</v>
       </c>
       <c r="C16" s="2">
-        <v>-2.684490485463122</v>
+        <v>-2.247765934191721</v>
       </c>
       <c r="D16" s="2">
-        <v>-12.74419526460708</v>
+        <v>-12.30822824251503</v>
       </c>
       <c r="E16" s="2">
-        <v>-11.5652301720163</v>
+        <v>-11.14457115230957</v>
       </c>
       <c r="F16" s="2">
-        <v>-14.76857453305526</v>
+        <v>-12.38491984390812</v>
       </c>
       <c r="G16" s="2">
-        <v>-13.24106316786271</v>
+        <v>-12.18134795111036</v>
       </c>
       <c r="H16" s="2">
-        <v>-16.08738102852206</v>
+        <v>-14.75879588234056</v>
       </c>
       <c r="I16" s="2">
-        <v>-14.29955186747264</v>
+        <v>-13.64782756674383</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2558,60 +2558,60 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="2">
-        <v>-11.49228677303553</v>
+        <v>-3.331051673610126</v>
       </c>
       <c r="C18" s="2">
-        <v>-5.952711599023645</v>
+        <v>-2.684490485463122</v>
       </c>
       <c r="D18" s="2">
-        <v>-18.386072879347</v>
+        <v>-12.74419526460708</v>
       </c>
       <c r="E18" s="2">
-        <v>-18.21090727542332</v>
+        <v>-11.5652301720163</v>
       </c>
       <c r="F18" s="2">
-        <v>-17.31428358578747</v>
+        <v>-14.76857453305526</v>
       </c>
       <c r="G18" s="2">
-        <v>-17.68145187335185</v>
+        <v>-13.24106316786271</v>
       </c>
       <c r="H18" s="2">
-        <v>-18.32582658070821</v>
+        <v>-16.08738102852206</v>
       </c>
       <c r="I18" s="2">
-        <v>-18.11341865651037</v>
+        <v>-14.29955186747264</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B19" s="2">
-        <v>-2.27054865275148</v>
+        <v>-11.49228677303553</v>
       </c>
       <c r="C19" s="2">
-        <v>-2.247765934191721</v>
+        <v>-5.952711599023645</v>
       </c>
       <c r="D19" s="2">
-        <v>-12.30822824251503</v>
+        <v>-18.386072879347</v>
       </c>
       <c r="E19" s="2">
-        <v>-11.14457115230957</v>
+        <v>-18.21090727542332</v>
       </c>
       <c r="F19" s="2">
-        <v>-12.38491984390812</v>
+        <v>-17.31428358578747</v>
       </c>
       <c r="G19" s="2">
-        <v>-12.18134795111036</v>
+        <v>-17.68145187335185</v>
       </c>
       <c r="H19" s="2">
-        <v>-14.75879588234056</v>
+        <v>-18.32582658070821</v>
       </c>
       <c r="I19" s="2">
-        <v>-13.64782756674383</v>
+        <v>-18.11341865651037</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2737,31 +2737,31 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2">
-        <v>0.4262577542033918</v>
+        <v>0.4361005523815438</v>
       </c>
       <c r="C26" s="2">
-        <v>0.2899430368587291</v>
+        <v>0.1843732446981761</v>
       </c>
       <c r="D26" s="2">
-        <v>0.600426353460308</v>
+        <v>0.1656435958141934</v>
       </c>
       <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0.07918333333333334</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0.07881666666666666</v>
+        <v>0.2415233567590648</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.3533865528603071</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I26" s="2">
-        <v>-4.22744006074679</v>
+        <v>-2.920691846838815</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2795,60 +2795,60 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2">
-        <v>0.1621415339290632</v>
+        <v>0.4262577542033918</v>
       </c>
       <c r="C28" s="2">
-        <v>0.05181635667822724</v>
+        <v>0.2899430368587291</v>
       </c>
       <c r="D28" s="2">
-        <v>0.1660303744910523</v>
+        <v>0.600426353460308</v>
       </c>
       <c r="E28" s="2">
-        <v>0.09591554596683807</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0.1807969282858515</v>
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G28" s="2">
-        <v>0.3746833333333333</v>
+        <v>0.07918333333333334</v>
       </c>
       <c r="H28" s="2">
-        <v>0.1556333333333333</v>
+        <v>0.07881666666666666</v>
       </c>
       <c r="I28" s="2">
-        <v>-319605180.2536416</v>
+        <v>-4.22744006074679</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2">
-        <v>0.4361005523815438</v>
+        <v>0.1621415339290632</v>
       </c>
       <c r="C29" s="2">
-        <v>0.1843732446981761</v>
+        <v>0.05181635667822724</v>
       </c>
       <c r="D29" s="2">
-        <v>0.1656435958141934</v>
+        <v>0.1660303744910523</v>
       </c>
       <c r="E29" s="2">
-        <v>0.2415233567590648</v>
+        <v>0.09591554596683807</v>
       </c>
       <c r="F29" s="2">
-        <v>0.3533865528603071</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>12</v>
+        <v>0.1807969282858515</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.3746833333333333</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.1556333333333333</v>
       </c>
       <c r="I29" s="2">
-        <v>-2.920691846838815</v>
+        <v>-319605180.2536416</v>
       </c>
     </row>
   </sheetData>
@@ -2928,25 +2928,25 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>-4.33</v>
+        <v>-5.63</v>
       </c>
       <c r="C4" s="2">
-        <v>-21.67</v>
+        <v>-3.69</v>
       </c>
       <c r="D4" s="2">
-        <v>-3.98</v>
+        <v>-8.109999999999999</v>
       </c>
       <c r="E4" s="2">
-        <v>-13.88</v>
+        <v>-4.31</v>
       </c>
       <c r="F4" s="2">
-        <v>-1.82</v>
+        <v>-3.43</v>
       </c>
       <c r="G4" s="2">
-        <v>-1.71</v>
+        <v>-2.19</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2974,94 +2974,94 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>-9.81</v>
+        <v>-4.33</v>
       </c>
       <c r="C6" s="2">
-        <v>-4.79</v>
+        <v>-21.67</v>
       </c>
       <c r="D6" s="2">
-        <v>-12.51</v>
+        <v>-3.98</v>
       </c>
       <c r="E6" s="2">
-        <v>-4.94</v>
+        <v>-13.88</v>
       </c>
       <c r="F6" s="2">
-        <v>-7.85</v>
+        <v>-1.82</v>
       </c>
       <c r="G6" s="2">
-        <v>-2.92</v>
+        <v>-1.71</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>-8.699999999999999</v>
+        <v>-2.86</v>
       </c>
       <c r="C7" s="2">
-        <v>-4.99</v>
+        <v>-11.26</v>
       </c>
       <c r="D7" s="2">
-        <v>-9.640000000000001</v>
+        <v>-3.41</v>
       </c>
       <c r="E7" s="2">
-        <v>-4.7</v>
+        <v>-3.2</v>
       </c>
       <c r="F7" s="2">
-        <v>-6.38</v>
+        <v>-1.68</v>
       </c>
       <c r="G7" s="2">
-        <v>-2.66</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>-2.86</v>
+        <v>-8.699999999999999</v>
       </c>
       <c r="C8" s="2">
-        <v>-11.26</v>
+        <v>-4.99</v>
       </c>
       <c r="D8" s="2">
-        <v>-3.41</v>
+        <v>-9.640000000000001</v>
       </c>
       <c r="E8" s="2">
-        <v>-3.2</v>
+        <v>-4.7</v>
       </c>
       <c r="F8" s="2">
-        <v>-1.68</v>
+        <v>-6.38</v>
       </c>
       <c r="G8" s="2">
-        <v>-1.79</v>
+        <v>-2.66</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>-5.63</v>
+        <v>-9.81</v>
       </c>
       <c r="C9" s="2">
-        <v>-3.69</v>
+        <v>-4.79</v>
       </c>
       <c r="D9" s="2">
-        <v>-8.109999999999999</v>
+        <v>-12.51</v>
       </c>
       <c r="E9" s="2">
-        <v>-4.31</v>
+        <v>-4.94</v>
       </c>
       <c r="F9" s="2">
-        <v>-3.43</v>
+        <v>-7.85</v>
       </c>
       <c r="G9" s="2">
-        <v>-2.19</v>
+        <v>-2.92</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3129,31 +3129,31 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2">
-        <v>-2.28</v>
+        <v>-2.56</v>
       </c>
       <c r="C14" s="2">
-        <v>-2.24</v>
+        <v>-2.31</v>
       </c>
       <c r="D14" s="2">
-        <v>-11.9</v>
+        <v>-14.2</v>
       </c>
       <c r="E14" s="2">
-        <v>-10.9</v>
+        <v>-12.6</v>
       </c>
       <c r="F14" s="2">
-        <v>-12.3</v>
+        <v>-13.4</v>
       </c>
       <c r="G14" s="2">
-        <v>-12.2</v>
+        <v>-12.7</v>
       </c>
       <c r="H14" s="2">
-        <v>-14.7</v>
+        <v>-16.5</v>
       </c>
       <c r="I14" s="2">
-        <v>-13.6</v>
+        <v>-14.8</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3187,118 +3187,118 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
-        <v>-8.109999999999999</v>
+        <v>-2.28</v>
       </c>
       <c r="C16" s="2">
-        <v>-4.63</v>
+        <v>-2.24</v>
       </c>
       <c r="D16" s="2">
-        <v>-17.7</v>
+        <v>-11.9</v>
       </c>
       <c r="E16" s="2">
-        <v>-14.9</v>
+        <v>-10.9</v>
       </c>
       <c r="F16" s="2">
-        <v>-17.6</v>
+        <v>-12.3</v>
       </c>
       <c r="G16" s="2">
-        <v>-17.8</v>
+        <v>-12.2</v>
       </c>
       <c r="H16" s="2">
-        <v>-18.2</v>
+        <v>-14.7</v>
       </c>
       <c r="I16" s="2">
-        <v>-18.1</v>
+        <v>-13.6</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2">
-        <v>-3.64</v>
+        <v>-2.31</v>
       </c>
       <c r="C17" s="2">
-        <v>-2.77</v>
+        <v>-2.27</v>
       </c>
       <c r="D17" s="2">
-        <v>-12.7</v>
+        <v>-11.2</v>
       </c>
       <c r="E17" s="2">
-        <v>-11.5</v>
+        <v>-10.7</v>
       </c>
       <c r="F17" s="2">
-        <v>-15</v>
+        <v>-12.3</v>
       </c>
       <c r="G17" s="2">
-        <v>-13.3</v>
+        <v>-12.3</v>
       </c>
       <c r="H17" s="2">
-        <v>-16</v>
+        <v>-14.7</v>
       </c>
       <c r="I17" s="2">
-        <v>-14.3</v>
+        <v>-14.2</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="2">
-        <v>-2.31</v>
+        <v>-3.64</v>
       </c>
       <c r="C18" s="2">
-        <v>-2.27</v>
+        <v>-2.77</v>
       </c>
       <c r="D18" s="2">
-        <v>-11.2</v>
+        <v>-12.7</v>
       </c>
       <c r="E18" s="2">
-        <v>-10.7</v>
+        <v>-11.5</v>
       </c>
       <c r="F18" s="2">
-        <v>-12.3</v>
+        <v>-15</v>
       </c>
       <c r="G18" s="2">
-        <v>-12.3</v>
+        <v>-13.3</v>
       </c>
       <c r="H18" s="2">
-        <v>-14.7</v>
+        <v>-16</v>
       </c>
       <c r="I18" s="2">
-        <v>-14.2</v>
+        <v>-14.3</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B19" s="2">
-        <v>-2.56</v>
+        <v>-8.109999999999999</v>
       </c>
       <c r="C19" s="2">
-        <v>-2.31</v>
+        <v>-4.63</v>
       </c>
       <c r="D19" s="2">
-        <v>-14.2</v>
+        <v>-17.7</v>
       </c>
       <c r="E19" s="2">
-        <v>-12.6</v>
+        <v>-14.9</v>
       </c>
       <c r="F19" s="2">
-        <v>-13.4</v>
+        <v>-17.6</v>
       </c>
       <c r="G19" s="2">
-        <v>-12.7</v>
+        <v>-17.8</v>
       </c>
       <c r="H19" s="2">
-        <v>-16.5</v>
+        <v>-18.2</v>
       </c>
       <c r="I19" s="2">
-        <v>-14.8</v>
+        <v>-18.1</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3366,31 +3366,31 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B24" s="2">
-        <v>0.414</v>
+        <v>0.601</v>
       </c>
       <c r="C24" s="2">
-        <v>0.121</v>
+        <v>0.391</v>
       </c>
       <c r="D24" s="2">
-        <v>0.185</v>
+        <v>0.672</v>
       </c>
       <c r="E24" s="2">
-        <v>0.27</v>
+        <v>0.324</v>
       </c>
       <c r="F24" s="2">
-        <v>0.384</v>
+        <v>0.528</v>
       </c>
       <c r="G24" s="2">
-        <v>0.117</v>
+        <v>0.394</v>
       </c>
       <c r="H24" s="2">
-        <v>0.081</v>
+        <v>0.371</v>
       </c>
       <c r="I24" s="2">
-        <v>-4.49</v>
+        <v>-0.43</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3424,118 +3424,118 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2">
-        <v>0.235</v>
+        <v>0.414</v>
       </c>
       <c r="C26" s="2">
-        <v>0.094</v>
+        <v>0.121</v>
       </c>
       <c r="D26" s="2">
-        <v>0</v>
+        <v>0.185</v>
       </c>
       <c r="E26" s="2">
-        <v>0.08199999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="F26" s="2">
-        <v>0.261</v>
+        <v>0.384</v>
       </c>
       <c r="G26" s="2">
-        <v>0.194</v>
+        <v>0.117</v>
       </c>
       <c r="H26" s="2">
-        <v>0.136</v>
+        <v>0.081</v>
       </c>
       <c r="I26" s="2">
-        <v>-6500000</v>
+        <v>-4.49</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2">
-        <v>0.4920000000000001</v>
+        <v>0.626</v>
       </c>
       <c r="C27" s="2">
-        <v>0.358</v>
+        <v>0.377</v>
       </c>
       <c r="D27" s="2">
-        <v>0.182</v>
+        <v>0.098</v>
       </c>
       <c r="E27" s="2">
-        <v>0</v>
+        <v>0.433</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>0.511</v>
       </c>
       <c r="G27" s="2">
-        <v>0.1</v>
+        <v>0.7929999999999999</v>
       </c>
       <c r="H27" s="2">
-        <v>0</v>
+        <v>0.794</v>
       </c>
       <c r="I27" s="2">
-        <v>-3.09</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2">
-        <v>0.626</v>
+        <v>0.4920000000000001</v>
       </c>
       <c r="C28" s="2">
-        <v>0.377</v>
+        <v>0.358</v>
       </c>
       <c r="D28" s="2">
-        <v>0.098</v>
+        <v>0.182</v>
       </c>
       <c r="E28" s="2">
-        <v>0.433</v>
+        <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>0.511</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>0.7929999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="2">
-        <v>0.794</v>
+        <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>-0.2</v>
+        <v>-3.09</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2">
-        <v>0.601</v>
+        <v>0.235</v>
       </c>
       <c r="C29" s="2">
-        <v>0.391</v>
+        <v>0.094</v>
       </c>
       <c r="D29" s="2">
-        <v>0.672</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2">
-        <v>0.324</v>
+        <v>0.08199999999999999</v>
       </c>
       <c r="F29" s="2">
-        <v>0.528</v>
+        <v>0.261</v>
       </c>
       <c r="G29" s="2">
-        <v>0.394</v>
+        <v>0.194</v>
       </c>
       <c r="H29" s="2">
-        <v>0.371</v>
+        <v>0.136</v>
       </c>
       <c r="I29" s="2">
-        <v>-0.43</v>
+        <v>-6500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>